<commit_message>
Excel und Benchmark angepasst
</commit_message>
<xml_diff>
--- a/latex/pdf2_phase2/Sql Benchmark.xlsx
+++ b/latex/pdf2_phase2/Sql Benchmark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilert\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weile\Desktop\Datenmanagement-jenseits-von-Relationen\latex\pdf2_phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF25B9A7-21FC-4D44-9888-C67557D2B0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A97CD-FE7D-4401-93C7-6193CEE4C322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A48560C7-F180-470A-8C32-AE93332693CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A48560C7-F180-470A-8C32-AE93332693CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="126">
   <si>
     <t>L</t>
   </si>
@@ -98,48 +98,6 @@
     <t>----- ----- -----</t>
   </si>
   <si>
-    <t>In 5 we got 392 calculations</t>
-  </si>
-  <si>
-    <t>In 4 we got 392 calculations</t>
-  </si>
-  <si>
-    <t>L: 10, Sparsity: 0.7999999999999999</t>
-  </si>
-  <si>
-    <t>Matrix in 355 ms</t>
-  </si>
-  <si>
-    <t>Array in 373 ms</t>
-  </si>
-  <si>
-    <t>A0 Finished in 379 ms</t>
-  </si>
-  <si>
-    <t>A1 Finished in 380 ms</t>
-  </si>
-  <si>
-    <t>A2 Finished in 386 ms</t>
-  </si>
-  <si>
-    <t>L: 10, Sparsity: 0.8999999999999999</t>
-  </si>
-  <si>
-    <t>Matrix in 397 ms</t>
-  </si>
-  <si>
-    <t>Array in 416 ms</t>
-  </si>
-  <si>
-    <t>A0 Finished in 421 ms</t>
-  </si>
-  <si>
-    <t>A1 Finished in 422 ms</t>
-  </si>
-  <si>
-    <t>A2 Finished in 428 ms</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -168,6 +126,294 @@
   </si>
   <si>
     <t>time in ms</t>
+  </si>
+  <si>
+    <t>Test 1: Extending size of Matrix:</t>
+  </si>
+  <si>
+    <t>L: 3, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 22 ms</t>
+  </si>
+  <si>
+    <t>Array in 53 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60001 ms 6710 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 130361 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60001 ms 174897 iterations</t>
+  </si>
+  <si>
+    <t>L: 4, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 46 ms</t>
+  </si>
+  <si>
+    <t>Array in 101 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60009 ms 4973 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 99311 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60001 ms 35006 iterations</t>
+  </si>
+  <si>
+    <t>L: 5, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 24 ms</t>
+  </si>
+  <si>
+    <t>Array in 86 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60010 ms 3450 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60003 ms 17924 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60009 ms 3434 iterations</t>
+  </si>
+  <si>
+    <t>L: 6, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>A0 in 60043 ms 1905 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60028 ms 1551 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60140 ms 225 iterations</t>
+  </si>
+  <si>
+    <t>L: 7, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 144 ms</t>
+  </si>
+  <si>
+    <t>Array in 376 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60133 ms 326 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60022 ms 133 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 61766 ms 31 iterations</t>
+  </si>
+  <si>
+    <t>L: 8, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 829 ms</t>
+  </si>
+  <si>
+    <t>Array in 1299 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60346 ms 71 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 63227 ms 17 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 66315 ms 4 iterations</t>
+  </si>
+  <si>
+    <t>L: 9, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Matrix in 3389 ms</t>
+  </si>
+  <si>
+    <t>Array in 4149 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60579 ms 17 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 102315 ms 2 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 126494 ms 1 iterations</t>
+  </si>
+  <si>
+    <t>Test 2: Extending Sparsity of Matrix:</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.1</t>
+  </si>
+  <si>
+    <t>Matrix in 96 ms</t>
+  </si>
+  <si>
+    <t>Array in 170 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60011 ms 4776 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 47363 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 33348 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.2</t>
+  </si>
+  <si>
+    <t>Matrix in 28 ms</t>
+  </si>
+  <si>
+    <t>Array in 61 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60012 ms 4993 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 52308 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60001 ms 33627 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.30000000000000004</t>
+  </si>
+  <si>
+    <t>Matrix in 25 ms</t>
+  </si>
+  <si>
+    <t>Array in 55 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60013 ms 5203 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 64005 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60001 ms 31215 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.4</t>
+  </si>
+  <si>
+    <t>Matrix in 37 ms</t>
+  </si>
+  <si>
+    <t>Array in 88 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60008 ms 4563 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 83547 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 33678 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.5</t>
+  </si>
+  <si>
+    <t>Array in 89 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60002 ms 5031 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 99150 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 32789 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.6</t>
+  </si>
+  <si>
+    <t>Matrix in 38 ms</t>
+  </si>
+  <si>
+    <t>Array in 70 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60012 ms 5285 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 112913 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 5107 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.7</t>
+  </si>
+  <si>
+    <t>Matrix in 18 ms</t>
+  </si>
+  <si>
+    <t>Array in 38 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60007 ms 5002 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 118510 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 35974 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.7999999999999999</t>
+  </si>
+  <si>
+    <t>Matrix in 26 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60003 ms 5135 iterations</t>
+  </si>
+  <si>
+    <t>A1 in 60001 ms 142890 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60002 ms 45015 iterations</t>
+  </si>
+  <si>
+    <t>L: 16, Sparsity: 0.8999999999999999</t>
+  </si>
+  <si>
+    <t>Matrix in 23 ms</t>
+  </si>
+  <si>
+    <t>Array in 58 ms</t>
+  </si>
+  <si>
+    <t>A0 in 60004 ms 5281 iterations</t>
+  </si>
+  <si>
+    <t>aA1 in 60001 ms 161128 iterations</t>
+  </si>
+  <si>
+    <t>A2 in 60001 ms 59150 iterations</t>
+  </si>
+  <si>
+    <t>Connection closed</t>
+  </si>
+  <si>
+    <t>Process finished with exit code 0</t>
   </si>
 </sst>
 </file>
@@ -224,9 +470,7 @@
         <color theme="4" tint="0.39997558519241921"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -235,9 +479,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -248,9 +490,7 @@
       <right style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -269,7 +509,46 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2008,7 +2287,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$18:$C$26</c:f>
+              <c:f>Tabelle1!$C$15:$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2043,7 +2322,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$18:$D$26</c:f>
+              <c:f>Tabelle1!$D$15:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2101,7 +2380,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$18:$C$26</c:f>
+              <c:f>Tabelle1!$C$15:$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2136,7 +2415,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$18:$E$26</c:f>
+              <c:f>Tabelle1!$E$15:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2471,7 +2750,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$F$18:$F$26</c:f>
+              <c:f>Tabelle1!$F$15:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2547,7 +2826,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$18:$G$26</c:f>
+              <c:f>Tabelle1!$G$15:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2951,7 +3230,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$18:$H$26</c:f>
+              <c:f>Tabelle1!$H$15:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3009,7 +3288,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$I$18:$I$26</c:f>
+              <c:f>Tabelle1!$I$15:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3067,7 +3346,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$J$18:$J$26</c:f>
+              <c:f>Tabelle1!$J$15:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -6806,6 +7085,24 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}" name="Tabelle2" displayName="Tabelle2" ref="B14:J23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="B14:J23" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{268488C2-A5FF-4022-A95A-A71A39B93066}" name="L"/>
+    <tableColumn id="2" xr3:uid="{1960BFD9-699C-41AE-9914-FFB4E1164DDE}" name="Sparsity"/>
+    <tableColumn id="3" xr3:uid="{C65E28CA-D021-46E8-B7AA-8C6CB863789E}" name="Matrix"/>
+    <tableColumn id="4" xr3:uid="{BAA4D170-4D75-4D65-B066-9D0F75DA292A}" name="Array"/>
+    <tableColumn id="5" xr3:uid="{31E62631-B5E3-40B7-A95D-FDE533AC32E5}" name="Multiplications"/>
+    <tableColumn id="6" xr3:uid="{8FD7C5A6-E59E-4310-AA80-94E61E6DB0B1}" name="time in ms"/>
+    <tableColumn id="7" xr3:uid="{7DC6EBD4-B4FB-468B-9644-92AE88E28492}" name="Calc_0"/>
+    <tableColumn id="8" xr3:uid="{5686A854-CFCA-4558-9359-D46360B50479}" name="Calc_1"/>
+    <tableColumn id="9" xr3:uid="{65DD080A-7AEB-47A8-96F3-B804D3198497}" name="Calc_2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -7123,25 +7420,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435958F5-8743-47F4-8342-B1B3508C5DBD}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
-      <selection activeCell="AA42" sqref="AA42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -7165,7 +7462,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -7195,7 +7495,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -7225,7 +7528,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -7255,7 +7561,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -7285,7 +7594,10 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -7315,7 +7627,10 @@
         <v>973</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -7345,7 +7660,10 @@
         <v>4792</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -7375,7 +7693,10 @@
         <v>34068</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -7405,7 +7726,10 @@
         <v>257860</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -7435,7 +7759,10 @@
         <v>2002741</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -7465,85 +7792,191 @@
         <v>15627092</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>44</v>
+      </c>
+      <c r="F15">
+        <v>392</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>52</v>
+      </c>
+      <c r="I15">
+        <v>52</v>
+      </c>
+      <c r="J15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>96</v>
+      </c>
+      <c r="F16">
+        <v>392</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>103</v>
+      </c>
+      <c r="I16">
+        <v>103</v>
+      </c>
+      <c r="J16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>130</v>
+      </c>
+      <c r="E17">
+        <v>150</v>
+      </c>
+      <c r="F17">
+        <v>392</v>
+      </c>
+      <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>156</v>
+      </c>
+      <c r="I17">
+        <v>157</v>
+      </c>
+      <c r="J17">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D18">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="E18">
-        <v>44</v>
+        <v>197</v>
       </c>
       <c r="F18">
         <v>392</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>52</v>
+        <v>203</v>
       </c>
       <c r="I18">
-        <v>52</v>
+        <v>203</v>
       </c>
       <c r="J18">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D19">
-        <v>73</v>
+        <v>222</v>
       </c>
       <c r="E19">
-        <v>96</v>
+        <v>243</v>
       </c>
       <c r="F19">
         <v>392</v>
@@ -7552,30 +7985,30 @@
         <v>6</v>
       </c>
       <c r="H19">
-        <v>103</v>
+        <v>250</v>
       </c>
       <c r="I19">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="J19">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>130</v>
+        <v>267</v>
       </c>
       <c r="E20">
-        <v>150</v>
+        <v>287</v>
       </c>
       <c r="F20">
         <v>392</v>
@@ -7584,243 +8017,553 @@
         <v>5</v>
       </c>
       <c r="H20">
-        <v>156</v>
+        <v>293</v>
       </c>
       <c r="I20">
-        <v>157</v>
+        <v>294</v>
       </c>
       <c r="J20">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>176</v>
+        <v>312</v>
       </c>
       <c r="E21">
-        <v>197</v>
+        <v>332</v>
       </c>
       <c r="F21">
         <v>392</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H21">
-        <v>203</v>
+        <v>339</v>
       </c>
       <c r="I21">
-        <v>203</v>
+        <v>339</v>
       </c>
       <c r="J21">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>222</v>
+        <v>355</v>
       </c>
       <c r="E22">
-        <v>243</v>
+        <v>373</v>
       </c>
       <c r="F22">
         <v>392</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>250</v>
+        <v>379</v>
       </c>
       <c r="I22">
-        <v>251</v>
+        <v>380</v>
       </c>
       <c r="J22">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>267</v>
+        <v>397</v>
       </c>
       <c r="E23">
-        <v>287</v>
+        <v>416</v>
       </c>
       <c r="F23">
         <v>392</v>
       </c>
       <c r="G23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>293</v>
+        <v>421</v>
       </c>
       <c r="I23">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="J23">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24">
-        <v>312</v>
-      </c>
-      <c r="E24">
-        <v>332</v>
-      </c>
-      <c r="F24">
-        <v>392</v>
-      </c>
-      <c r="G24">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>339</v>
-      </c>
-      <c r="I24">
-        <v>339</v>
-      </c>
-      <c r="J24">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <v>355</v>
-      </c>
-      <c r="E25">
-        <v>373</v>
-      </c>
-      <c r="F25">
-        <v>392</v>
-      </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25">
-        <v>379</v>
-      </c>
-      <c r="I25">
-        <v>380</v>
-      </c>
-      <c r="J25">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26">
-        <v>397</v>
-      </c>
-      <c r="E26">
-        <v>416</v>
-      </c>
-      <c r="F26">
-        <v>392</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-      <c r="H26">
-        <v>421</v>
-      </c>
-      <c r="I26">
-        <v>422</v>
-      </c>
-      <c r="J26">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A2 Finito P2 Finito
</commit_message>
<xml_diff>
--- a/latex/pdf2_phase2/Sql Benchmark.xlsx
+++ b/latex/pdf2_phase2/Sql Benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weilert\Desktop\Datenmanagement-jenseits-von-Relationen\latex\pdf2_phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2AE664-8A5D-40F0-B170-C81E5F2F4059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF50A27-30A3-41EF-A07B-CB1015E439F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A48560C7-F180-470A-8C32-AE93332693CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>L</t>
   </si>
@@ -83,9 +83,6 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>----- ----- -----</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -114,87 +111,6 @@
   </si>
   <si>
     <t>time in ms</t>
-  </si>
-  <si>
-    <t>L: 16, Sparsity: 0.5</t>
-  </si>
-  <si>
-    <t>L: 16, Sparsity: 0.6</t>
-  </si>
-  <si>
-    <t>L: 16, Sparsity: 0.7</t>
-  </si>
-  <si>
-    <t>L: 16, Sparsity: 0.7999999999999999</t>
-  </si>
-  <si>
-    <t>L: 16, Sparsity: 0.8999999999999999</t>
-  </si>
-  <si>
-    <t>Connection closed</t>
-  </si>
-  <si>
-    <t>Process finished with exit code 0</t>
-  </si>
-  <si>
-    <t>Matrix in 13 ms</t>
-  </si>
-  <si>
-    <t>A0 in 60002 ms 7858 iterations</t>
-  </si>
-  <si>
-    <t>Array in 30 ms</t>
-  </si>
-  <si>
-    <t>Array in 31 ms</t>
-  </si>
-  <si>
-    <t>A0 in 60004 ms 7812 iterations</t>
-  </si>
-  <si>
-    <t>A1 in 60001 ms 167380 iterations</t>
-  </si>
-  <si>
-    <t>A2 in 60001 ms 54081 iterations</t>
-  </si>
-  <si>
-    <t>A0 in 60004 ms 7797 iterations</t>
-  </si>
-  <si>
-    <t>A1 in 60001 ms 191930 iterations</t>
-  </si>
-  <si>
-    <t>A2 in 60001 ms 55799 iterations</t>
-  </si>
-  <si>
-    <t>A1 in 60001 ms 238197 iterations</t>
-  </si>
-  <si>
-    <t>A2 in 60001 ms 60804 iterations</t>
-  </si>
-  <si>
-    <t>Matrix in 12 ms</t>
-  </si>
-  <si>
-    <t>Array in 29 ms</t>
-  </si>
-  <si>
-    <t>A0 in 60008 ms 7786 iterations</t>
-  </si>
-  <si>
-    <t>A1 in 60001 ms 233777 iterations</t>
-  </si>
-  <si>
-    <t>A2 in 60001 ms 72239 iterations</t>
-  </si>
-  <si>
-    <t>A0 in 60005 ms 7822 iterations</t>
-  </si>
-  <si>
-    <t>A1 in 60001 ms 274409 iterations</t>
-  </si>
-  <si>
-    <t>A2 in 60001 ms 88414 iterations</t>
   </si>
 </sst>
 </file>
@@ -493,7 +409,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$2:$B$9</c:f>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -525,7 +441,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$9</c:f>
+              <c:f>Tabelle1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -637,7 +553,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$2:$B$9</c:f>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -669,7 +585,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$2:$E$9</c:f>
+              <c:f>Tabelle1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1040,7 +956,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$2:$B$9</c:f>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1072,7 +988,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$9</c:f>
+              <c:f>Tabelle1!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1184,7 +1100,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$2:$B$9</c:f>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1216,7 +1132,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$2:$H$9</c:f>
+              <c:f>Tabelle1!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1328,7 +1244,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$2:$B$9</c:f>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1360,7 +1276,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$I$2:$I$9</c:f>
+              <c:f>Tabelle1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1719,7 +1635,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$13:$C$21</c:f>
+              <c:f>Tabelle1!$B$13:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1754,7 +1670,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$13:$D$21</c:f>
+              <c:f>Tabelle1!$C$13:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1869,7 +1785,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$13:$C$21</c:f>
+              <c:f>Tabelle1!$B$13:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1904,7 +1820,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$13:$E$21</c:f>
+              <c:f>Tabelle1!$D$13:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2278,7 +2194,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$13:$C$21</c:f>
+              <c:f>Tabelle1!$B$13:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2313,7 +2229,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$13:$G$21</c:f>
+              <c:f>Tabelle1!$F$13:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2428,7 +2344,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$13:$C$21</c:f>
+              <c:f>Tabelle1!$B$13:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2463,7 +2379,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$13:$H$21</c:f>
+              <c:f>Tabelle1!$G$13:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2578,7 +2494,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$C$13:$C$21</c:f>
+              <c:f>Tabelle1!$B$13:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2613,7 +2529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$I$13:$I$21</c:f>
+              <c:f>Tabelle1!$H$13:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -5084,13 +5000,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>523874</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -5120,13 +5036,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -5156,13 +5072,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>323849</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -5194,13 +5110,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -5234,8 +5150,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36182CDF-E5D7-47B1-9A7C-B125D47352E3}" name="Tabelle1" displayName="Tabelle1" ref="B1:I9" totalsRowShown="0">
-  <autoFilter ref="B1:I9" xr:uid="{36182CDF-E5D7-47B1-9A7C-B125D47352E3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36182CDF-E5D7-47B1-9A7C-B125D47352E3}" name="Tabelle1" displayName="Tabelle1" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9" xr:uid="{36182CDF-E5D7-47B1-9A7C-B125D47352E3}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A665FDCF-B5C4-4971-A406-F8CE27A9D810}" name="L"/>
     <tableColumn id="2" xr3:uid="{6B5B30ED-4C69-4E8A-91F4-BB5B864F6034}" name="Sparsity"/>
@@ -5251,8 +5167,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}" name="Tabelle2" displayName="Tabelle2" ref="B12:I21" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="B12:I21" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}" name="Tabelle2" displayName="Tabelle2" ref="A12:H21" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A12:H21" xr:uid="{D9EE2641-B875-4987-B7E4-5092C28E792B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{268488C2-A5FF-4022-A95A-A71A39B93066}" name="L"/>
     <tableColumn id="2" xr3:uid="{1960BFD9-699C-41AE-9914-FFB4E1164DDE}" name="Sparsity"/>
@@ -5584,653 +5500,510 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435958F5-8743-47F4-8342-B1B3508C5DBD}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC22" sqref="AC22"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>60001</v>
+      </c>
+      <c r="F2">
+        <v>11150</v>
+      </c>
+      <c r="G2">
+        <v>217409</v>
+      </c>
+      <c r="H2">
+        <v>266703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>60005</v>
+      </c>
+      <c r="F3">
+        <v>7613</v>
+      </c>
+      <c r="G3">
+        <v>168847</v>
+      </c>
+      <c r="H3">
+        <v>54244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>39</v>
+      </c>
+      <c r="E4">
+        <v>60001</v>
+      </c>
+      <c r="F4">
+        <v>4555</v>
+      </c>
+      <c r="G4">
+        <v>32822</v>
+      </c>
+      <c r="H4">
+        <v>8158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>63</v>
+      </c>
+      <c r="E5">
+        <v>60012</v>
+      </c>
+      <c r="F5">
+        <v>2672</v>
+      </c>
+      <c r="G5">
+        <v>5320</v>
+      </c>
+      <c r="H5">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>127</v>
+      </c>
+      <c r="D6">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>60017</v>
+      </c>
+      <c r="F6">
+        <v>1060</v>
+      </c>
+      <c r="G6">
+        <v>685</v>
+      </c>
+      <c r="H6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>206</v>
+      </c>
+      <c r="D7">
+        <v>331</v>
+      </c>
+      <c r="E7">
+        <v>60381</v>
+      </c>
+      <c r="F7">
+        <v>255</v>
+      </c>
+      <c r="G7">
+        <v>85</v>
+      </c>
+      <c r="H7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>916</v>
+      </c>
+      <c r="D8">
+        <v>1259</v>
+      </c>
+      <c r="E8">
+        <v>60377</v>
+      </c>
+      <c r="F8">
+        <v>57</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>4204</v>
+      </c>
+      <c r="D9">
+        <v>5546</v>
+      </c>
+      <c r="E9">
+        <v>60063</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>45</v>
+      </c>
+      <c r="E13">
+        <v>60001</v>
+      </c>
+      <c r="F13">
+        <v>7770</v>
+      </c>
+      <c r="G13">
+        <v>86315</v>
+      </c>
+      <c r="H13">
+        <v>53220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E14">
+        <v>60001</v>
+      </c>
+      <c r="F14">
+        <v>7762</v>
+      </c>
+      <c r="G14">
+        <v>96711</v>
+      </c>
+      <c r="H14">
+        <v>52879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>60001</v>
+      </c>
+      <c r="F15">
+        <v>7858</v>
+      </c>
+      <c r="G15">
+        <v>114706</v>
+      </c>
+      <c r="H15">
+        <v>52930</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>60001</v>
+      </c>
+      <c r="F16">
+        <v>7766</v>
+      </c>
+      <c r="G16">
+        <v>144902</v>
+      </c>
+      <c r="H16">
+        <v>53380</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <v>38</v>
-      </c>
-      <c r="F2">
-        <v>60001</v>
-      </c>
-      <c r="G2">
-        <v>11150</v>
-      </c>
-      <c r="H2">
-        <v>217409</v>
-      </c>
-      <c r="I2">
-        <v>266703</v>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>31</v>
+      </c>
+      <c r="E17">
+        <v>60002</v>
+      </c>
+      <c r="F17">
+        <v>7812</v>
+      </c>
+      <c r="G17">
+        <v>167380</v>
+      </c>
+      <c r="H17">
+        <v>54081</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
         <v>13</v>
       </c>
-      <c r="E3">
-        <v>35</v>
-      </c>
-      <c r="F3">
+      <c r="D18">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <v>60002</v>
+      </c>
+      <c r="F18">
+        <v>7797</v>
+      </c>
+      <c r="G18">
+        <v>191930</v>
+      </c>
+      <c r="H18">
+        <v>55799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>31</v>
+      </c>
+      <c r="E19">
+        <v>60002</v>
+      </c>
+      <c r="F19">
+        <v>7858</v>
+      </c>
+      <c r="G19">
+        <v>238197</v>
+      </c>
+      <c r="H19">
+        <v>60804</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>60002</v>
+      </c>
+      <c r="F20">
+        <v>7786</v>
+      </c>
+      <c r="G20">
+        <v>233777</v>
+      </c>
+      <c r="H20">
+        <v>72239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21">
         <v>60005</v>
       </c>
-      <c r="G3">
-        <v>7613</v>
-      </c>
-      <c r="H3">
-        <v>168847</v>
-      </c>
-      <c r="I3">
-        <v>54244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>39</v>
-      </c>
-      <c r="F4">
-        <v>60001</v>
-      </c>
-      <c r="G4">
-        <v>4555</v>
-      </c>
-      <c r="H4">
-        <v>32822</v>
-      </c>
-      <c r="I4">
-        <v>8158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>63</v>
-      </c>
-      <c r="F5">
-        <v>60012</v>
-      </c>
-      <c r="G5">
-        <v>2672</v>
-      </c>
-      <c r="H5">
-        <v>5320</v>
-      </c>
-      <c r="I5">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>127</v>
-      </c>
-      <c r="E6">
-        <v>65</v>
-      </c>
-      <c r="F6">
-        <v>60017</v>
-      </c>
-      <c r="G6">
-        <v>1060</v>
-      </c>
-      <c r="H6">
-        <v>685</v>
-      </c>
-      <c r="I6">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>206</v>
-      </c>
-      <c r="E7">
-        <v>331</v>
-      </c>
-      <c r="F7">
-        <v>60381</v>
-      </c>
-      <c r="G7">
-        <v>255</v>
-      </c>
-      <c r="H7">
-        <v>85</v>
-      </c>
-      <c r="I7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8">
-        <v>916</v>
-      </c>
-      <c r="E8">
-        <v>1259</v>
-      </c>
-      <c r="F8">
-        <v>60377</v>
-      </c>
-      <c r="G8">
-        <v>57</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9">
-        <v>4204</v>
-      </c>
-      <c r="E9">
-        <v>5546</v>
-      </c>
-      <c r="F9">
-        <v>60063</v>
-      </c>
-      <c r="G9">
-        <v>12</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>19</v>
-      </c>
-      <c r="E13">
-        <v>45</v>
-      </c>
-      <c r="F13">
-        <v>60001</v>
-      </c>
-      <c r="G13">
-        <v>7770</v>
-      </c>
-      <c r="H13">
-        <v>86315</v>
-      </c>
-      <c r="I13">
-        <v>53220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14">
-        <v>15</v>
-      </c>
-      <c r="E14">
-        <v>33</v>
-      </c>
-      <c r="F14">
-        <v>60001</v>
-      </c>
-      <c r="G14">
-        <v>7762</v>
-      </c>
-      <c r="H14">
-        <v>96711</v>
-      </c>
-      <c r="I14">
-        <v>52879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
-      </c>
-      <c r="E15">
-        <v>32</v>
-      </c>
-      <c r="F15">
-        <v>60001</v>
-      </c>
-      <c r="G15">
-        <v>7858</v>
-      </c>
-      <c r="H15">
-        <v>114706</v>
-      </c>
-      <c r="I15">
-        <v>52930</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>13</v>
-      </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-      <c r="F16">
-        <v>60001</v>
-      </c>
-      <c r="G16">
-        <v>7766</v>
-      </c>
-      <c r="H16">
-        <v>144902</v>
-      </c>
-      <c r="I16">
-        <v>53380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>13</v>
-      </c>
-      <c r="E17">
-        <v>31</v>
-      </c>
-      <c r="F17">
-        <v>60002</v>
-      </c>
-      <c r="G17">
-        <v>7812</v>
-      </c>
-      <c r="H17">
-        <v>167380</v>
-      </c>
-      <c r="I17">
-        <v>54081</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>13</v>
-      </c>
-      <c r="E18">
-        <v>31</v>
-      </c>
-      <c r="F18">
-        <v>60002</v>
-      </c>
-      <c r="G18">
-        <v>7797</v>
-      </c>
-      <c r="H18">
-        <v>191930</v>
-      </c>
-      <c r="I18">
-        <v>55799</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>13</v>
-      </c>
-      <c r="E19">
-        <v>31</v>
-      </c>
-      <c r="F19">
-        <v>60002</v>
-      </c>
-      <c r="G19">
-        <v>7858</v>
-      </c>
-      <c r="H19">
-        <v>238197</v>
-      </c>
-      <c r="I19">
-        <v>60804</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20">
-        <v>12</v>
-      </c>
-      <c r="E20">
-        <v>29</v>
-      </c>
-      <c r="F20">
-        <v>60002</v>
-      </c>
-      <c r="G20">
-        <v>7786</v>
-      </c>
-      <c r="H20">
-        <v>233777</v>
-      </c>
-      <c r="I20">
-        <v>72239</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21">
-        <v>13</v>
-      </c>
-      <c r="E21">
-        <v>30</v>
-      </c>
       <c r="F21">
-        <v>60005</v>
+        <v>7822</v>
       </c>
       <c r="G21">
-        <v>7822</v>
+        <v>274409</v>
       </c>
       <c r="H21">
-        <v>274409</v>
-      </c>
-      <c r="I21">
         <v>88414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>